<commit_message>
feat (plugin): convert support strict array
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="97">
   <si>
     <t>level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -376,6 +376,22 @@
   </si>
   <si>
     <t>$strict [</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ghost{</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rr</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -714,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BD10"/>
+  <dimension ref="A2:BG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="BA8" sqref="BA8"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="BC14" sqref="BC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,16 +777,19 @@
     <col min="50" max="50" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="51" max="52" width="2" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="2" customWidth="1"/>
-    <col min="55" max="55" width="3.6640625" customWidth="1"/>
-    <col min="56" max="56" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="6.33203125" customWidth="1"/>
+    <col min="56" max="56" width="2" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="2" customWidth="1"/>
+    <col min="58" max="58" width="3.6640625" customWidth="1"/>
+    <col min="59" max="59" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="3.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -781,7 +800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -792,7 +811,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>7</v>
       </c>
@@ -938,22 +957,31 @@
         <v>11</v>
       </c>
       <c r="AZ5" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="BA5" t="s">
         <v>90</v>
       </c>
       <c r="BB5" t="s">
+        <v>93</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>94</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>92</v>
+      </c>
+      <c r="BE5" t="s">
         <v>89</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BF5" t="s">
         <v>14</v>
       </c>
-      <c r="BD5" t="s">
+      <c r="BG5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>24</v>
       </c>
@@ -1011,11 +1039,14 @@
       <c r="AX6" t="s">
         <v>83</v>
       </c>
-      <c r="BD6" t="s">
+      <c r="BC6">
+        <v>1</v>
+      </c>
+      <c r="BG6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.2">
       <c r="D7">
         <v>20</v>
       </c>
@@ -1071,11 +1102,14 @@
       <c r="AU7">
         <v>111</v>
       </c>
-      <c r="BD7">
+      <c r="BA7">
         <v>1</v>
       </c>
+      <c r="BG7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.2">
       <c r="D8">
         <v>20</v>
       </c>
@@ -1136,11 +1170,14 @@
       <c r="BA8">
         <v>2</v>
       </c>
-      <c r="BD8">
+      <c r="BC8">
         <v>2</v>
       </c>
+      <c r="BG8">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.2">
       <c r="D9">
         <v>20</v>
       </c>
@@ -1192,11 +1229,14 @@
       <c r="BA9">
         <v>3</v>
       </c>
-      <c r="BD9">
+      <c r="BC9" t="s">
+        <v>95</v>
+      </c>
+      <c r="BG9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.2">
       <c r="D10">
         <v>20</v>
       </c>
@@ -1248,7 +1288,10 @@
       <c r="BA10">
         <v>2</v>
       </c>
-      <c r="BD10">
+      <c r="BC10">
+        <v>3</v>
+      </c>
+      <c r="BG10">
         <v>2</v>
       </c>
     </row>

</xml_diff>